<commit_message>
added encoder and phototransistor links from discord into the need to order file
</commit_message>
<xml_diff>
--- a/Need to order.xlsx
+++ b/Need to order.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/ryan_laur_ufl_edu/Documents/Projects/laser_harp/github/laser-harp-midi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anony\Documents\GitHub\laser-harp-midi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B85183E0-694F-4E49-91B8-E3CBE3F3F685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FC4CBD-5BD2-4617-B814-B4600162C5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6F0DA424-F3AD-4469-88B4-39D442433476}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{6F0DA424-F3AD-4469-88B4-39D442433476}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,54 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Encoder</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Bourns/PAC18R1-43D19F?qs=IS%252B4QmGtzzoiPnRwlkZJXA%3D%3D</t>
+  </si>
+  <si>
+    <t>Phototransistors</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-semiconductor-opto-division/TEPT5700/1681193</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -62,13 +104,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -381,12 +427,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D4E9C6-B901-4629-8C63-A0F84F77941B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="14.04296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" tooltip="https://www.mouser.com/ProductDetail/Bourns/PAC18R1-43D19F?qs=IS%252B4QmGtzzoiPnRwlkZJXA%3D%3D" xr:uid="{F19DBF8D-A714-424C-B40A-593B74407EF9}"/>
+    <hyperlink ref="C3" r:id="rId2" tooltip="https://www.digikey.com/en/products/detail/vishay-semiconductor-opto-division/TEPT5700/1681193" xr:uid="{573A9A02-DADB-4D46-8A9B-E607776FECC8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>